<commit_message>
🐞&️🧩: Finish the function of insert CSV, including the condition that source files exist.
</commit_message>
<xml_diff>
--- a/src/test/resources/insert_pkg/Student.xlsx
+++ b/src/test/resources/insert_pkg/Student.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1280" uniqueCount="56">
   <si>
     <t>joe:1575181630689</t>
   </si>
@@ -53,6 +53,135 @@
   </si>
   <si>
     <t>joe:1575181709787</t>
+  </si>
+  <si>
+    <t>joe:1575182976960</t>
+  </si>
+  <si>
+    <t>joe:1575182976961</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>joe:1575182977146</t>
+  </si>
+  <si>
+    <t>joe:1575182979206</t>
+  </si>
+  <si>
+    <t>joe:1575182979320</t>
+  </si>
+  <si>
+    <t>joe:1575182979392</t>
+  </si>
+  <si>
+    <t>joe:1575182979393</t>
+  </si>
+  <si>
+    <t>joe:1575185100527</t>
+  </si>
+  <si>
+    <t>joe:1575185100528</t>
+  </si>
+  <si>
+    <t>joe:1575185100737</t>
+  </si>
+  <si>
+    <t>joe:1575185103124</t>
+  </si>
+  <si>
+    <t>joe:1575185103249</t>
+  </si>
+  <si>
+    <t>joe:1575185103344</t>
+  </si>
+  <si>
+    <t>joe:1575186447159</t>
+  </si>
+  <si>
+    <t>joe:1575186447160</t>
+  </si>
+  <si>
+    <t>joe:1575186447390</t>
+  </si>
+  <si>
+    <t>joe:1575186449457</t>
+  </si>
+  <si>
+    <t>joe:1575186449563</t>
+  </si>
+  <si>
+    <t>joe:1575186449659</t>
+  </si>
+  <si>
+    <t>joe:1575792715489</t>
+  </si>
+  <si>
+    <t>2019/12/08</t>
+  </si>
+  <si>
+    <t>joe:1575792715727</t>
+  </si>
+  <si>
+    <t>joe:1575792717744</t>
+  </si>
+  <si>
+    <t>joe:1575792717745</t>
+  </si>
+  <si>
+    <t>joe:1575792717845</t>
+  </si>
+  <si>
+    <t>joe:1575792718070</t>
+  </si>
+  <si>
+    <t>joe:1577605746807</t>
+  </si>
+  <si>
+    <t>2019/12/29</t>
+  </si>
+  <si>
+    <t>joe:1577605746808</t>
+  </si>
+  <si>
+    <t>joe:1577605747032</t>
+  </si>
+  <si>
+    <t>joe:1577605748874</t>
+  </si>
+  <si>
+    <t>joe:1577605748963</t>
+  </si>
+  <si>
+    <t>joe:1577605749031</t>
+  </si>
+  <si>
+    <t>joe:1577605749032</t>
   </si>
 </sst>
 </file>
@@ -97,7 +226,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -139,7 +268,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -151,12 +280,165 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
@@ -168,12 +450,165 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>3</v>
+      </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
@@ -185,7 +620,160 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>48</v>
+      </c>
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>18</v>
+      </c>
+      <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" t="s">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>48</v>
+      </c>
+      <c r="B44" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" t="s">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -195,17 +783,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="20.0" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="20.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -227,7 +815,7 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -239,7 +827,160 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -249,7 +990,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -257,7 +998,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -269,7 +1010,160 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>